<commit_message>
Add comprehensive beef extraction evaluation framework with LangSmith integration, 9 datasets, and complete documentation
</commit_message>
<xml_diff>
--- a/data/incoming/beef_cuts.xlsx
+++ b/data/incoming/beef_cuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Desktop/GitHub/Cluster_AI/data/incoming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E04DF51-F72C-5E4E-93A2-90C5E24F61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EA07F57-A07D-1C41-82C1-3143057751E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="176">
   <si>
     <t>Sub-primal</t>
   </si>
@@ -88,18 +88,54 @@
     <t>Blade Meat</t>
   </si>
   <si>
-    <t>Scotch Tender</t>
-  </si>
-  <si>
-    <t>Mock Tender</t>
-  </si>
-  <si>
     <t>Official / Commercial Grade Name</t>
   </si>
   <si>
     <t>Common Synonyms &amp; Acronyms</t>
   </si>
   <si>
+    <t>USDA Prime</t>
+  </si>
+  <si>
+    <t>USDA Choice</t>
+  </si>
+  <si>
+    <t>USDA Select</t>
+  </si>
+  <si>
+    <t>USDA Standard</t>
+  </si>
+  <si>
+    <t>USDA Commercial</t>
+  </si>
+  <si>
+    <t>USDA Utility</t>
+  </si>
+  <si>
+    <t>USDA Cutter</t>
+  </si>
+  <si>
+    <t>USDA Canner</t>
+  </si>
+  <si>
+    <r>
+      <t>No-Roll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Ungraded)</t>
+    </r>
+  </si>
+  <si>
+    <t>(Other) Angus Brands</t>
+  </si>
+  <si>
     <t>Wagyu / Kobe</t>
   </si>
   <si>
@@ -115,6 +151,12 @@
     <t>NR, Ungraded, Unstamped</t>
   </si>
   <si>
+    <t>CAB, Certified Angus</t>
+  </si>
+  <si>
+    <t>Angus, Creekstone Angus, CAB Prime</t>
+  </si>
+  <si>
     <t>Wagyu, Kobe Beef, A5 (JP scale)</t>
   </si>
   <si>
@@ -133,12 +175,12 @@
     <t>Utility, Ut, B4 (bulls), Canad Utility, B grades</t>
   </si>
   <si>
+    <t>Certified Angus Beef</t>
+  </si>
+  <si>
     <t>Inside Round</t>
   </si>
   <si>
-    <t>Top Round, Inside Round (CAN)</t>
-  </si>
-  <si>
     <t>Outside Round</t>
   </si>
   <si>
@@ -205,6 +247,9 @@
     <t>Chuck Eye Roll</t>
   </si>
   <si>
+    <t>Clod Shoulder Roast</t>
+  </si>
+  <si>
     <t>Clod Heart (center muscle)</t>
   </si>
   <si>
@@ -229,18 +274,15 @@
     <t>Chuck Blade Meat, Cap &amp; Wedge</t>
   </si>
   <si>
-    <t>Mock Tender, Chuck Tender</t>
-  </si>
-  <si>
     <t>Clod Roast</t>
   </si>
   <si>
+    <t>ScottyTender</t>
+  </si>
+  <si>
     <t>Flank Steak</t>
   </si>
   <si>
-    <t>London Broil (prep), Jiffy Steak, Falda (MEX)</t>
-  </si>
-  <si>
     <t>Flank Fillet</t>
   </si>
   <si>
@@ -310,9 +352,6 @@
     <t>Ball Tip</t>
   </si>
   <si>
-    <t>Sirloin Tip Roast (sirloin)</t>
-  </si>
-  <si>
     <t>Sirloin Flap</t>
   </si>
   <si>
@@ -529,50 +568,29 @@
     <t>Pre-cut Fajita Beef</t>
   </si>
   <si>
-    <t>Prime</t>
-  </si>
-  <si>
-    <t>Choice</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>Utility</t>
-  </si>
-  <si>
-    <t>Cutter</t>
-  </si>
-  <si>
-    <t>Canner</t>
-  </si>
-  <si>
-    <t>Scotty Tender</t>
-  </si>
-  <si>
-    <t>Clod Shoulder Roast, Shoulder Clod</t>
-  </si>
-  <si>
-    <t>Angus</t>
-  </si>
-  <si>
-    <t>Angus, Creekstone Angus, CAB Prime, Certified Angus Beef, CAB, Certified Angus</t>
-  </si>
-  <si>
-    <t>No-Roll</t>
+    <t>aka Ball tip 2/up or 2/dn</t>
+  </si>
+  <si>
+    <t>a shell is a bone in striploin</t>
+  </si>
+  <si>
+    <t>Scotch Tender, Mock Tender, Chuck Tender</t>
+  </si>
+  <si>
+    <t>Jiffy Steak, Falda (MEX)</t>
+  </si>
+  <si>
+    <t>Top Round, Inside Round (CAN), London Broil (prep)</t>
+  </si>
+  <si>
+    <t>Sirloin Tip Roast (sirloin), Ball tip 2/up, or 2/dn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +610,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -658,6 +683,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1B7491-B904-0943-99A3-71255300AAE5}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
@@ -978,100 +1005,108 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>163</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>173</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>171</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1103,34 +1138,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1162,138 +1197,138 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1305,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J18:J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1325,34 +1360,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1400,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1388,50 +1423,50 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1444,12 +1479,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1465,42 +1500,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1511,10 +1546,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,7 +1558,7 @@
     <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1535,123 +1570,116 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1660,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1700,7 @@
     <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1680,20 +1708,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1703,19 +1732,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1723,68 +1752,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1817,44 +1853,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1888,34 +1924,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1947,42 +1983,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in batch processing
</commit_message>
<xml_diff>
--- a/data/incoming/beef_cuts.xlsx
+++ b/data/incoming/beef_cuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Desktop/GitHub/Cluster_AI/data/incoming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EA07F57-A07D-1C41-82C1-3143057751E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93497DFD-973D-EB49-AA95-5375EA0ADD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="175">
   <si>
     <t>Sub-primal</t>
   </si>
@@ -566,9 +566,6 @@
   </si>
   <si>
     <t>Pre-cut Fajita Beef</t>
-  </si>
-  <si>
-    <t>aka Ball tip 2/up or 2/dn</t>
   </si>
   <si>
     <t>a shell is a bone in striploin</t>
@@ -670,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -684,7 +681,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -1426,7 +1422,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1526,7 +1522,7 @@
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1667,11 +1663,11 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>172</v>
+      <c r="B14" t="s">
+        <v>171</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1713,7 +1709,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -1734,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1760,7 +1756,7 @@
         <v>88</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1800,12 +1796,10 @@
         <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Integrate working API connection and add MCP setup
- Rebased onto full-pipeline-working branch with working API connection
- Added Databricks MCP setup documentation and test script
- Added caching system for Firebase data filtering
- Resolved conflicts by accepting all changes from full-pipeline-working branch
</commit_message>
<xml_diff>
--- a/data/incoming/beef_cuts.xlsx
+++ b/data/incoming/beef_cuts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billnewman/Desktop/GitHub/Cluster_AI/data/incoming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015479D9-1119-7E4D-818D-E61AACB4A987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6557EB8C-E4AE-8247-B5C1-1A13700FABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="175">
   <si>
     <t>Sub-primal</t>
   </si>
@@ -86,12 +86,6 @@
   </si>
   <si>
     <t>Blade Meat</t>
-  </si>
-  <si>
-    <t>Scotch Tender</t>
-  </si>
-  <si>
-    <t>Mock Tender</t>
   </si>
   <si>
     <t>Official / Commercial Grade Name</t>
@@ -187,9 +181,6 @@
     <t>Inside Round</t>
   </si>
   <si>
-    <t>Top Round, Inside Round (CAN)</t>
-  </si>
-  <si>
     <t>Outside Round</t>
   </si>
   <si>
@@ -283,9 +274,6 @@
     <t>Chuck Blade Meat, Cap &amp; Wedge</t>
   </si>
   <si>
-    <t>Mock Tender, Chuck Tender</t>
-  </si>
-  <si>
     <t>Clod Roast</t>
   </si>
   <si>
@@ -295,9 +283,6 @@
     <t>Flank Steak</t>
   </si>
   <si>
-    <t>London Broil (prep), Jiffy Steak, Falda (MEX)</t>
-  </si>
-  <si>
     <t>Flank Fillet</t>
   </si>
   <si>
@@ -367,9 +352,6 @@
     <t>Ball Tip</t>
   </si>
   <si>
-    <t>Sirloin Tip Roast (sirloin)</t>
-  </si>
-  <si>
     <t>Sirloin Flap</t>
   </si>
   <si>
@@ -584,13 +566,28 @@
   </si>
   <si>
     <t>Pre-cut Fajita Beef</t>
+  </si>
+  <si>
+    <t>a shell is a bone in striploin</t>
+  </si>
+  <si>
+    <t>Scotch Tender, Mock Tender, Chuck Tender</t>
+  </si>
+  <si>
+    <t>Jiffy Steak, Falda (MEX)</t>
+  </si>
+  <si>
+    <t>Top Round, Inside Round (CAN), London Broil (prep)</t>
+  </si>
+  <si>
+    <t>Sirloin Tip Roast (sirloin), Ball tip 2/up, or 2/dn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,6 +607,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -670,13 +674,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,10 +988,10 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
@@ -997,108 +1001,108 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1124,40 +1128,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1170,7 +1174,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="B3" sqref="B3:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1183,144 +1187,144 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1332,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J18:J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1346,40 +1350,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1396,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1407,58 +1411,58 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1471,12 +1475,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1484,50 +1488,50 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1538,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A16:B16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,11 +1554,11 @@
     <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
@@ -1562,118 +1566,116 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>171</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1682,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1694,28 +1696,29 @@
     <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1725,88 +1728,93 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>98</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>100</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1833,50 +1841,50 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1889,7 +1897,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D5"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1904,40 +1912,40 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +1958,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1963,48 +1971,48 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>